<commit_message>
Final commit for the semester
Various board changes.
</commit_message>
<xml_diff>
--- a/Schematics/Rocket Control Board/Version-5/Parts/Parts.xlsx
+++ b/Schematics/Rocket Control Board/Version-5/Parts/Parts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>100nF</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>ABS25-32.768KHZ-6-1-T</t>
+  </si>
+  <si>
+    <t>WHERE IS THE REGULATOR</t>
   </si>
 </sst>
 </file>
@@ -663,10 +666,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="H8:L8"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1069,6 +1072,11 @@
         <v>13.129999999999999</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1079,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>